<commit_message>
Power Supply Reqs added to excel
</commit_message>
<xml_diff>
--- a/PinList.xlsx
+++ b/PinList.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\VisionCore-FPGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E8945C5-E0F0-4EA5-B0B6-69A0DE8E0F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B50105-E2F1-46BE-A232-6517F00D0925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0A8F01DE-F7E1-4584-9986-24437E6C4AF7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0A8F01DE-F7E1-4584-9986-24437E6C4AF7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All pins" sheetId="1" r:id="rId1"/>
+    <sheet name="Power supply" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4145" uniqueCount="1384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4171" uniqueCount="1393">
   <si>
     <t>Pin</t>
   </si>
@@ -4188,14 +4189,63 @@
   </si>
   <si>
     <t>T18</t>
+  </si>
+  <si>
+    <t>Absolute maximum ratings</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CC_PSINTFP</t>
+    </r>
+  </si>
+  <si>
+    <t>PS primary logic full-power domain supply voltage</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="5">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -4207,13 +4257,36 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4228,10 +4301,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4567,10 +4659,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5DFCA2-99FE-4B5E-9F69-9F39E0B8A59B}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.499984740745262"/>
+  </sheetPr>
   <dimension ref="B1:G785"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A557" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C710" sqref="A579:C710"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D564" sqref="D564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20281,4 +20376,201 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25216EC2-EFD7-413D-8C3E-E87141EEDF9B}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75">
+      <c r="A1" s="7" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1387</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18">
+      <c r="A3" s="4" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="E13" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="E14" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="E15" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="3"/>
+      <c r="E16" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="3"/>
+      <c r="E17" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="E18" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="E19" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="E20" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the PinList spreadsheet and added a GNS block and DDR block for FPGA
</commit_message>
<xml_diff>
--- a/PinList.xlsx
+++ b/PinList.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\VisionCore-FPGA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srdjan.milkic\Desktop\VisionCore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B50105-E2F1-46BE-A232-6517F00D0925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007E393F-C48F-4D75-88DB-59FCDF616E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0A8F01DE-F7E1-4584-9986-24437E6C4AF7}"/>
+    <workbookView xWindow="11610" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{0A8F01DE-F7E1-4584-9986-24437E6C4AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="All pins" sheetId="1" r:id="rId1"/>
-    <sheet name="Power supply" sheetId="3" r:id="rId2"/>
+    <sheet name="Absolute maximum ratings" sheetId="3" r:id="rId2"/>
+    <sheet name="Recommended Operating Condition" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4171" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4465" uniqueCount="1551">
   <si>
     <t>Pin</t>
   </si>
@@ -4191,9 +4192,6 @@
     <t>T18</t>
   </si>
   <si>
-    <t>Absolute maximum ratings</t>
-  </si>
-  <si>
     <t>Symbol</t>
   </si>
   <si>
@@ -4206,7 +4204,307 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Unit</t>
+    <t>PS primary logic full-power domain supply voltage</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>PS auxiliary supply voltage</t>
+  </si>
+  <si>
+    <t>PS DDR controller and PHY supply voltage</t>
+  </si>
+  <si>
+    <t>PS SYSMON ADC supply voltage relative to GND_PSADC</t>
+  </si>
+  <si>
+    <t>PS PLL supply voltage</t>
+  </si>
+  <si>
+    <t>PS-GTR supply voltage</t>
+  </si>
+  <si>
+    <t>PS-GTR termination voltage</t>
+  </si>
+  <si>
+    <t>PS-GTR reference clock input voltage</t>
+  </si>
+  <si>
+    <t>PS-GTR receiver input voltage</t>
+  </si>
+  <si>
+    <t>PS DDR I/O supply voltage</t>
+  </si>
+  <si>
+    <t>PS DDR PLL supply voltage</t>
+  </si>
+  <si>
+    <t>PS I/O supply</t>
+  </si>
+  <si>
+    <t>PS I/O input voltage</t>
+  </si>
+  <si>
+    <t>PS DDR I/O input voltage</t>
+  </si>
+  <si>
+    <t>PS battery-backed RAM and battery-backed real-time clock (RTC) supply voltage</t>
+  </si>
+  <si>
+    <t>PS full-power domain supply voltage</t>
+  </si>
+  <si>
+    <t>For -3E devices: PS full-power domain supply voltage</t>
+  </si>
+  <si>
+    <t>PS low-power domain supply voltage</t>
+  </si>
+  <si>
+    <t>For -3E devices: PS low-power domain supply voltage</t>
+  </si>
+  <si>
+    <t>VCC_PSINTFP_DDR 3</t>
+  </si>
+  <si>
+    <t>For -3E devices: PS DDR controller and PHY supply voltage</t>
+  </si>
+  <si>
+    <t>VCC_PSINTFP 3</t>
+  </si>
+  <si>
+    <t>VPS_MGTRAVCC 4</t>
+  </si>
+  <si>
+    <t>VPS_MGTRAVTT 4</t>
+  </si>
+  <si>
+    <t>VCCO_PSDDR 5</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>VCCO_PSIO 6</t>
+  </si>
+  <si>
+    <t>–0.200</t>
+  </si>
+  <si>
+    <t>VCC_PSBATT 7</t>
+  </si>
+  <si>
+    <t>Programmable Logic</t>
+  </si>
+  <si>
+    <t>PL internal supply voltage</t>
+  </si>
+  <si>
+    <t>For -3E devices: PL internal supply voltage</t>
+  </si>
+  <si>
+    <t>VCCINT_IO 8</t>
+  </si>
+  <si>
+    <t>PL internal supply voltage for the I/O banks</t>
+  </si>
+  <si>
+    <t>For -3E devices: PL internal supply voltage for the I/O banks</t>
+  </si>
+  <si>
+    <t>VCCBRAM 8</t>
+  </si>
+  <si>
+    <t>Block RAM and UltraRAM supply voltage</t>
+  </si>
+  <si>
+    <t>For -3E devices: block RAM and UltraRAM supply voltage</t>
+  </si>
+  <si>
+    <t>VCCAUX 11</t>
+  </si>
+  <si>
+    <t>Auxiliary supply voltage</t>
+  </si>
+  <si>
+    <t>Supply voltage for HD I/O banks 9</t>
+  </si>
+  <si>
+    <t>Supply voltage for HP I/O banks 10</t>
+  </si>
+  <si>
+    <t>VCCAUX_IO 11</t>
+  </si>
+  <si>
+    <t>Auxiliary I/O supply voltage</t>
+  </si>
+  <si>
+    <t>I/O input voltage</t>
+  </si>
+  <si>
+    <t>IIN 14</t>
+  </si>
+  <si>
+    <t>Maximum current through any PL or PS pin in a powered or unpowered bank when forward biasing the clamp diode</t>
+  </si>
+  <si>
+    <t>mA</t>
+  </si>
+  <si>
+    <t>GTH or GTY Transceiver</t>
+  </si>
+  <si>
+    <t>VMGTAVCC 15</t>
+  </si>
+  <si>
+    <t>Analog supply voltage for the GTH or GTY transceiver</t>
+  </si>
+  <si>
+    <t>VMGTAVTT 15</t>
+  </si>
+  <si>
+    <t>Analog supply voltage for the GTH or GTY transmitter and receiver termination circuits</t>
+  </si>
+  <si>
+    <t>VMGTVCCAUX 15</t>
+  </si>
+  <si>
+    <t>Auxiliary analog QPLL voltage supply for the transceivers</t>
+  </si>
+  <si>
+    <t>VMGTAVTTRCAL 15</t>
+  </si>
+  <si>
+    <t>Analog supply voltage for the resistor calibration circuit of the GTH or GTY transceiver column</t>
+  </si>
+  <si>
+    <t>VCU</t>
+  </si>
+  <si>
+    <t>Internal supply voltage for the VCU</t>
+  </si>
+  <si>
+    <t>PL System Monitor</t>
+  </si>
+  <si>
+    <t>PL System Monitor supply relative to GNDADC</t>
+  </si>
+  <si>
+    <t>PL System Monitor externally supplied reference voltage relative to GNDADC</t>
+  </si>
+  <si>
+    <t>Description 1</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Processor System (PS)</t>
+  </si>
+  <si>
+    <t>–0.500</t>
+  </si>
+  <si>
+    <t>PS primary logic low-power domain supply voltage</t>
+  </si>
+  <si>
+    <t>VPSIN 2</t>
+  </si>
+  <si>
+    <t>Programmable Logic (PL)</t>
+  </si>
+  <si>
+    <t>Internal supply voltage</t>
+  </si>
+  <si>
+    <t>VCCINT_IO 3</t>
+  </si>
+  <si>
+    <t>Internal supply voltage for the I/O banks</t>
+  </si>
+  <si>
+    <t>VCCAUX 4</t>
+  </si>
+  <si>
+    <t>VCCBRAM 3</t>
+  </si>
+  <si>
+    <t>Supply voltage for the block RAM and UltraRAM</t>
+  </si>
+  <si>
+    <t>Output drivers supply voltage for HD I/O banks</t>
+  </si>
+  <si>
+    <t>Output drivers supply voltage for HP I/O banks</t>
+  </si>
+  <si>
+    <t>VCCAUX_IO 4</t>
+  </si>
+  <si>
+    <t>Auxiliary supply voltage for the I/O banks</t>
+  </si>
+  <si>
+    <t>Input reference voltage for HP I/O banks</t>
+  </si>
+  <si>
+    <t>I/O input voltage for HD I/O banks</t>
+  </si>
+  <si>
+    <t>–0.550</t>
+  </si>
+  <si>
+    <t>I/O input voltage for HP I/O banks</t>
+  </si>
+  <si>
+    <t>Available output current at the pad</t>
+  </si>
+  <si>
+    <t>–20</t>
+  </si>
+  <si>
+    <t>Available RMS output current at the pad</t>
+  </si>
+  <si>
+    <t>GTH or GTY Transceiver 8</t>
+  </si>
+  <si>
+    <t>Analog supply voltage for transceiver circuits</t>
+  </si>
+  <si>
+    <t>Analog supply voltage for transceiver termination circuits</t>
+  </si>
+  <si>
+    <t>Auxiliary analog Quad PLL (QPLL) voltage supply for transceivers</t>
+  </si>
+  <si>
+    <t>Transceiver reference clock absolute input voltage</t>
+  </si>
+  <si>
+    <t>Analog supply voltage for the resistor calibration circuit of the transceiver column</t>
+  </si>
+  <si>
+    <t>Receiver (RXP/RXN) and transmitter (TXP/TXN) absolute input voltage</t>
+  </si>
+  <si>
+    <t>DC input current for receiver input pins DC coupled RX termination = floating 9</t>
+  </si>
+  <si>
+    <t>DC input current for receiver input pins DC coupled RX termination = GND 10</t>
+  </si>
+  <si>
+    <t>DC input current for receiver input pins DC coupled RX termination = programmable 11</t>
+  </si>
+  <si>
+    <t>DC output current for transmitter pins DC coupled RX termination = floating</t>
+  </si>
+  <si>
+    <t>Video Codec Unit</t>
+  </si>
+  <si>
+    <t>Internal supply voltage for the video codec unit</t>
+  </si>
+  <si>
+    <t>PL System Monitor reference input relative to GNDADC</t>
   </si>
   <si>
     <r>
@@ -4214,29 +4512,990 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>CC_PSINTFP</t>
     </r>
   </si>
   <si>
-    <t>PS primary logic full-power domain supply voltage</t>
-  </si>
-  <si>
-    <t>V</t>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSINTLP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSAUX</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSINTFP_DDR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSADC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSPLL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PS_MGTRAVCC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PS_MGTRAVTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PS_MGTREFCLK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PS_MGTRIN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO_PSDDR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSDDR_PLL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO_PSIO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO_PSIO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + 0.550</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO_PSDDR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + 0.550</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSBATT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>REF</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2, 5, 6 , 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + 0.550</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>RMS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MGTAVCC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MGTAVTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MGTVCCAUX</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MGTREFCLK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MGTAVTTRCAL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>IN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DCIN-FLOAT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DCIN-MGTAVTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DC input current for receiver input pins DC coupled RX termination = V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MGTAVTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DCIN-GND</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DCIN-PROG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DCOUT-FLOAT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DCOUT-MGTAVTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DC output current for transmitter pins DC coupled RX termination = V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MGTAVTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT_VCU</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCADC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>REFP</t>
+    </r>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>Processor System</t>
+  </si>
+  <si>
+    <r>
+      <t>For -1LI and -2LE (V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> = 0.72V) devices: PS full-power domain supply voltage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSINTLP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For -1LI and -2LE (V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> = 0.72V) devices: PS low-power domain supply voltage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSAUX</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For -1LI and -2LE (V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> = 0.72V) devices: PS DDR controller and PHY supply voltage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSADC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSPLL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CC_PSDDR_PLL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PSIN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO_PSIO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + 0.200</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO_PSDDR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + 0.200</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For -1LI and -2LE (V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> = 0.72V) devices: PL internal supply voltage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For -1LI and -2LE (V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> = 0.72V) devices: PL internal supply voltage for the I/O banks</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>12, 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + 0.200</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCINT_VCU</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCADC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>REFP</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4259,23 +5518,81 @@
     </font>
     <font>
       <b/>
-      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.89999084444715716"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="2"/>
+      <sz val="10"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4288,8 +5605,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -4297,33 +5638,844 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4668,9 +6820,9 @@
       <selection activeCell="D564" sqref="D564"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
@@ -20381,195 +22533,1722 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25216EC2-EFD7-413D-8C3E-E87141EEDF9B}">
   <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:H49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A35" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="74.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1">
+      <c r="A1" s="51" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="7" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D5" s="15">
+        <v>2</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="12" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="12" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D7" s="15">
+        <v>2</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1.32</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="12" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="12" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="12" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="12" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="12" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1.65</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="12" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D14" s="15">
+        <v>2</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="12" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D15" s="15">
+        <v>3.63</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="17" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>1502</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="26.4">
+      <c r="A17" s="17"/>
+      <c r="B17" s="13" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1">
+      <c r="A18" s="19" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D18" s="22">
+        <v>2</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1">
+      <c r="A19" s="4" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="24" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D20" s="26">
+        <v>1</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1">
+      <c r="A21" s="28" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D21" s="18">
+        <v>1</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="28" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D22" s="18">
+        <v>2</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="28" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D23" s="18">
+        <v>1</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="30" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D24" s="18">
+        <v>3.4</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>1389</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="31"/>
+      <c r="B25" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D25" s="18">
+        <v>2</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="28" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D26" s="18">
+        <v>2</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="32" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D27" s="18">
+        <v>2</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="30" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="31"/>
+      <c r="B29" s="13" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="32" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D30" s="18">
+        <v>20</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1">
+      <c r="A31" s="33" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D31" s="35">
+        <v>20</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" thickBot="1">
+      <c r="A32" s="37" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="39"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="24" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D33" s="26">
+        <v>1</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="32" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D34" s="18">
+        <v>1.3</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="32" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D35" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="32" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1.3</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="32" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1.3</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="32" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="32" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D39" s="18">
+        <v>10</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="32" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D40" s="18">
+        <v>10</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="32" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D41" s="18">
+        <v>0</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="32" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D42" s="18">
+        <v>0</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="32" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D43" s="18">
+        <v>6</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" thickBot="1">
+      <c r="A44" s="33" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D44" s="35">
+        <v>6</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" thickBot="1">
+      <c r="A45" s="41" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="43"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1">
+      <c r="A46" s="44" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B46" s="45" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D46" s="47">
+        <v>1</v>
+      </c>
+      <c r="E46" s="47" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1">
+      <c r="A47" s="41" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="43"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="48" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D48" s="26">
+        <v>2</v>
+      </c>
+      <c r="E48" s="50" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1">
+      <c r="A49" s="19" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D49" s="35">
+        <v>2</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A16:A17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F7FC18-974D-41C3-8586-1935356FF433}">
+  <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="55" customWidth="1"/>
+    <col min="2" max="2" width="74.44140625" style="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="60" t="s">
         <v>1384</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="61" t="s">
         <v>1385</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C1" s="62" t="s">
         <v>1386</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D1" s="62" t="s">
+        <v>1529</v>
+      </c>
+      <c r="E1" s="62" t="s">
         <v>1387</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>1388</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F1" s="63" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1">
+      <c r="A2" s="64" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="65"/>
+    </row>
+    <row r="3" spans="1:6" ht="40.200000000000003" customHeight="1">
+      <c r="A3" s="68" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B3" s="77" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C3" s="86">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="D3" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E3" s="86">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F3" s="93" t="s">
         <v>1389</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:6" ht="21" customHeight="1">
+      <c r="A4" s="68"/>
+      <c r="B4" s="78" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C4" s="87">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="D4" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E4" s="87">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F4" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21.6" customHeight="1">
+      <c r="A5" s="68"/>
+      <c r="B5" s="78" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C5" s="87">
+        <v>0.873</v>
+      </c>
+      <c r="D5" s="81">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="87">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F5" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="67" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B6" s="78" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C6" s="87">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="D6" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="87">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F6" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="67"/>
+      <c r="B7" s="78" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C7" s="87">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="D7" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="87">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F7" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="67"/>
+      <c r="B8" s="78" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C8" s="87">
+        <v>0.873</v>
+      </c>
+      <c r="D8" s="81">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="87">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F8" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="70" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B9" s="78" t="s">
         <v>1390</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C9" s="87">
+        <v>1.71</v>
+      </c>
+      <c r="D9" s="81">
+        <v>1.8</v>
+      </c>
+      <c r="E9" s="87">
+        <v>1.89</v>
+      </c>
+      <c r="F9" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="68" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B10" s="78" t="s">
         <v>1391</v>
       </c>
-      <c r="C3" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="C10" s="87">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="D10" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E10" s="87">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F10" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="68"/>
+      <c r="B11" s="78" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C11" s="87">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="D11" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E11" s="87">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F11" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="68"/>
+      <c r="B12" s="78" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C12" s="87">
+        <v>0.873</v>
+      </c>
+      <c r="D12" s="81">
+        <v>0.9</v>
+      </c>
+      <c r="E12" s="87">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F12" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="70" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B13" s="78" t="s">
         <v>1392</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="E13" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="E14" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="E15" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16" s="3"/>
-      <c r="E16" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="3"/>
-      <c r="E17" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="E18" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="E19" s="8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="E20" s="8" t="s">
-        <v>1392</v>
+      <c r="C13" s="87">
+        <v>1.71</v>
+      </c>
+      <c r="D13" s="81">
+        <v>1.8</v>
+      </c>
+      <c r="E13" s="87">
+        <v>1.89</v>
+      </c>
+      <c r="F13" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="70" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B14" s="78" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C14" s="87">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="D14" s="81">
+        <v>1.2</v>
+      </c>
+      <c r="E14" s="87">
+        <v>1.236</v>
+      </c>
+      <c r="F14" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="69" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B15" s="78" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C15" s="87">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D15" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E15" s="87">
+        <v>0.875</v>
+      </c>
+      <c r="F15" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="69" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B16" s="78" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C16" s="87">
+        <v>1.746</v>
+      </c>
+      <c r="D16" s="81">
+        <v>1.8</v>
+      </c>
+      <c r="E16" s="87">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="F16" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="69" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B17" s="78" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C17" s="87">
+        <v>1.06</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E17" s="87">
+        <v>1.575</v>
+      </c>
+      <c r="F17" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="70" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B18" s="78" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C18" s="87">
+        <v>1.71</v>
+      </c>
+      <c r="D18" s="81">
+        <v>1.8</v>
+      </c>
+      <c r="E18" s="87">
+        <v>1.89</v>
+      </c>
+      <c r="F18" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="69" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C19" s="87">
+        <v>1.71</v>
+      </c>
+      <c r="D19" s="81" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E19" s="87">
+        <v>3.4649999999999999</v>
+      </c>
+      <c r="F19" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="26.4">
+      <c r="A20" s="67" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B20" s="78" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C20" s="87" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D20" s="81" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E20" s="96" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F20" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="39.6">
+      <c r="A21" s="67"/>
+      <c r="B21" s="78" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C21" s="87" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D21" s="81" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E21" s="96" t="s">
+        <v>1541</v>
+      </c>
+      <c r="F21" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1">
+      <c r="A22" s="71" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B22" s="80" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C22" s="88">
+        <v>1.2</v>
+      </c>
+      <c r="D22" s="82" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E22" s="88">
+        <v>1.5</v>
+      </c>
+      <c r="F22" s="94" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1">
+      <c r="A23" s="56" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="58"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="90" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B24" s="77" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C24" s="83">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D24" s="86">
+        <v>0.85</v>
+      </c>
+      <c r="E24" s="83">
+        <v>0.876</v>
+      </c>
+      <c r="F24" s="86" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="67"/>
+      <c r="B25" s="78" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C25" s="81">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="D25" s="87">
+        <v>0.72</v>
+      </c>
+      <c r="E25" s="81">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="F25" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="67"/>
+      <c r="B26" s="78" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C26" s="81">
+        <v>0.873</v>
+      </c>
+      <c r="D26" s="87">
+        <v>0.9</v>
+      </c>
+      <c r="E26" s="81">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F26" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="68" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B27" s="78" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C27" s="81">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D27" s="87">
+        <v>0.85</v>
+      </c>
+      <c r="E27" s="81">
+        <v>0.876</v>
+      </c>
+      <c r="F27" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="68"/>
+      <c r="B28" s="78" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C28" s="81">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D28" s="87">
+        <v>0.85</v>
+      </c>
+      <c r="E28" s="81">
+        <v>0.876</v>
+      </c>
+      <c r="F28" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="68"/>
+      <c r="B29" s="78" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C29" s="81">
+        <v>0.873</v>
+      </c>
+      <c r="D29" s="87">
+        <v>0.9</v>
+      </c>
+      <c r="E29" s="81">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F29" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="68" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B30" s="78" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C30" s="81">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D30" s="87">
+        <v>0.85</v>
+      </c>
+      <c r="E30" s="81">
+        <v>0.876</v>
+      </c>
+      <c r="F30" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="68"/>
+      <c r="B31" s="78" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C31" s="81">
+        <v>0.873</v>
+      </c>
+      <c r="D31" s="87">
+        <v>0.9</v>
+      </c>
+      <c r="E31" s="81">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F31" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="69" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B32" s="78" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C32" s="81">
+        <v>1.746</v>
+      </c>
+      <c r="D32" s="87">
+        <v>1.8</v>
+      </c>
+      <c r="E32" s="81">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="F32" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="67" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B33" s="79" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C33" s="81">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="D33" s="87" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E33" s="81">
+        <v>3.4</v>
+      </c>
+      <c r="F33" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="67"/>
+      <c r="B34" s="79" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C34" s="81">
+        <v>0.95</v>
+      </c>
+      <c r="D34" s="87" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E34" s="81">
+        <v>1.9</v>
+      </c>
+      <c r="F34" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="69" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B35" s="78" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C35" s="81">
+        <v>1.746</v>
+      </c>
+      <c r="D35" s="87">
+        <v>1.8</v>
+      </c>
+      <c r="E35" s="81">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="F35" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="26.4">
+      <c r="A36" s="70" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B36" s="78" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C36" s="81" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D36" s="87" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E36" s="81" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F36" s="87" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="27" thickBot="1">
+      <c r="A37" s="71" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B37" s="80" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C37" s="82" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D37" s="88" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E37" s="82">
+        <v>10</v>
+      </c>
+      <c r="F37" s="88" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" thickBot="1">
+      <c r="A38" s="56" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="58"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="72" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B39" s="77" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C39" s="86">
+        <v>0.873</v>
+      </c>
+      <c r="D39" s="83">
+        <v>0.9</v>
+      </c>
+      <c r="E39" s="86">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F39" s="92" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="69" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B40" s="78" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C40" s="87">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="D40" s="81">
+        <v>1.2</v>
+      </c>
+      <c r="E40" s="87">
+        <v>1.236</v>
+      </c>
+      <c r="F40" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="69" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B41" s="78" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C41" s="87">
+        <v>1.746</v>
+      </c>
+      <c r="D41" s="81">
+        <v>1.8</v>
+      </c>
+      <c r="E41" s="87">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="F41" s="93" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="27" thickBot="1">
+      <c r="A42" s="71" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B42" s="80" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C42" s="88">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="D42" s="82">
+        <v>1.2</v>
+      </c>
+      <c r="E42" s="88">
+        <v>1.236</v>
+      </c>
+      <c r="F42" s="94" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" thickBot="1">
+      <c r="A43" s="56" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="58"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" thickBot="1">
+      <c r="A44" s="73" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B44" s="91" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C44" s="84">
+        <v>0.873</v>
+      </c>
+      <c r="D44" s="89">
+        <v>0.9</v>
+      </c>
+      <c r="E44" s="76">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F44" s="66" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15" thickBot="1">
+      <c r="A45" s="56" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="58"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="74" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B46" s="77" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C46" s="83">
+        <v>1.746</v>
+      </c>
+      <c r="D46" s="86">
+        <v>1.8</v>
+      </c>
+      <c r="E46" s="83">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="F46" s="86" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" thickBot="1">
+      <c r="A47" s="75" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B47" s="80" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C47" s="85">
+        <v>1.2</v>
+      </c>
+      <c r="D47" s="88">
+        <v>1.25</v>
+      </c>
+      <c r="E47" s="85">
+        <v>1.3</v>
+      </c>
+      <c r="F47" s="88" t="s">
+        <v>1389</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="13">
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>